<commit_message>
Poprawki, automatyczne nadawanie nazw plikow
</commit_message>
<xml_diff>
--- a/WzoryUslug/Intermista.xlsx
+++ b/WzoryUslug/Intermista.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" codeName="Ten_skoroszyt"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503C5E3E-8346-430A-B5BD-78BA3EB52CB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD9EA54-500D-4039-B062-FCF685E0CE9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Imię</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Internista</t>
+  </si>
+  <si>
+    <t>Notatki</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,6 +248,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -531,10 +537,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Arkusz1"/>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K24" sqref="J24:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,24 +623,127 @@
       <c r="B11" s="6"/>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A14:D31"/>
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>